<commit_message>
Updates with day corrected
</commit_message>
<xml_diff>
--- a/results/in_house/C. albicans.xlsx
+++ b/results/in_house/C. albicans.xlsx
@@ -491,7 +491,7 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C5" t="n">
         <v>10</v>
@@ -504,7 +504,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C6" t="n">
         <v>10</v>
@@ -517,7 +517,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C7" t="n">
         <v>10</v>

</xml_diff>